<commit_message>
meetings page shows list of appointments
</commit_message>
<xml_diff>
--- a/Gantt Charts/Milestone3-GanttChart.xlsx
+++ b/Gantt Charts/Milestone3-GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shana/Desktop/CMPE 131/calApp/Calendar-Scheduling-App-master/Gantt Charts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF6EC7D-112A-2442-B6A3-7008F3384565}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA1EFB4-87A6-DD43-912B-288335E51988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="26920" windowHeight="17480" xr2:uid="{AA7B69DF-3B17-C04C-9150-938323FE9379}"/>
   </bookViews>
@@ -272,7 +272,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +317,12 @@
     <fill>
       <patternFill patternType="lightUp">
         <fgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -581,7 +587,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -746,6 +752,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -1080,7 +1089,7 @@
   <dimension ref="A1:BN175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1494,13 +1503,17 @@
       <c r="C6" s="8">
         <v>3</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="29">
+        <v>43948</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="47"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1568,15 +1581,19 @@
       <c r="C7" s="8">
         <v>3</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="29">
+        <v>43948</v>
+      </c>
+      <c r="E7" s="8">
+        <v>5</v>
+      </c>
       <c r="F7" s="9"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1710,12 +1727,16 @@
       <c r="C9" s="8">
         <v>3</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="8"/>
+      <c r="D9" s="29">
+        <v>43948</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="47"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1784,13 +1805,17 @@
       <c r="C10" s="8">
         <v>3</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="29">
+        <v>43948</v>
+      </c>
+      <c r="E10" s="8">
+        <v>3</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1858,13 +1883,17 @@
       <c r="C11" s="8">
         <v>3</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="29">
+        <v>43948</v>
+      </c>
+      <c r="E11" s="8">
+        <v>3</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1932,13 +1961,17 @@
       <c r="C12" s="8">
         <v>3</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="29">
+        <v>43948</v>
+      </c>
+      <c r="E12" s="8">
+        <v>3</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -2074,15 +2107,19 @@
       <c r="C14" s="8">
         <v>2</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="29">
+        <v>43951</v>
+      </c>
+      <c r="E14" s="8">
+        <v>2</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -2148,15 +2185,19 @@
       <c r="C15" s="8">
         <v>2</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="29">
+        <v>43952</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
+      <c r="L15" s="24"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -3450,11 +3491,11 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="C3:C4" xr:uid="{9EF1E97C-CF64-7948-A8CD-EA30BA312303}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="B3:B4" xr:uid="{8971EE31-53FE-6F44-A4E7-A0061F08C39F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="A3:A4" xr:uid="{DE19D017-F753-9340-9B91-166526B028E1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="P2" xr:uid="{AF31CE32-1CA2-014D-AD02-59BB94C6851E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="P2 K7:L7" xr:uid="{AF31CE32-1CA2-014D-AD02-59BB94C6851E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="L2" xr:uid="{6DD34810-F035-CA45-BE1C-F3677A0D3BFA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="M2 I2 G5:H5" xr:uid="{DB1E9FAD-1F0C-9A4B-A530-B1B2314CD711}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="M2 I2 G5:H5 J10:J12 H9:I12 L14:L15 K14 H6" xr:uid="{DB1E9FAD-1F0C-9A4B-A530-B1B2314CD711}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="F2" xr:uid="{2BAFCFB1-7B74-E646-8171-7AC2A48CCDBF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="H6:I6 C2" xr:uid="{B12D7A5D-6678-2247-9E84-D505C287109C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="C2" xr:uid="{B12D7A5D-6678-2247-9E84-D505C287109C}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>